<commit_message>
Get daily reddit data: Tue Jan 30 08:07:51 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_04.xlsx
+++ b/data/2024_02_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C457"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2658 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1aej3x4</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>so proud of them, the favs I ever did 🥰</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aej3x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1aei4sh</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Completely obsessed with these nails I’m so sad to change :(</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uizwvyyzwifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1aei0d6</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>I NEED to stop biting my nails, HELP 🥲</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97gil1fmvifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1aehatl</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>This is your reminder to TREAT YOSELF!</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b55kn1tonifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1aegxsm</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>I love my set. Thinking pink next time</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6sxnajxjifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1aegkv3</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Manicure options without filing?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aegkv3/manicure_options_without_filing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1aegnfx</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Not usually a pink fan but 😍</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7gpketlgifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1aefyy6</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Couldn’t decide between pink or red.</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0cbg097aifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1aebsyt</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>been doing my nails for roughly a year now, what do we think?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3luclyf9hfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ae7o5g</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Which shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae7o5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1aef8h9</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Press on nail myths/misconceptions</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aef8h9/press_on_nail_mythsmisconceptions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1aeekhg</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Weird smell from using nail dril</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aeekhg/weird_smell_from_using_nail_dril/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1aedvgr</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>black pearl coquette 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oieercsyqhfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1aed6le</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>A little purple to get me through the end of January 🪻💜 Rubber base gel + gel colour + water decal done by me on my natural nails</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlpc9a43lhfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1aecyos</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>First time doing my own gel-x</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvu9e8k6jhfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1aecxpf</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Do you ask for $$ when practicing on friends??</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aecxpf/do_you_ask_for_when_practicing_on_friends/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1aecsmv</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Uv light activated vs air activated nail prep</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aecsmv/uv_light_activated_vs_air_activated_nail_prep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1aec3xa</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>A year later</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aec3xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1aebut6</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Nothing special but I’ve always had a hard time growing my nails out n I just think they look v pretty 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcv7aglu9hfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1aeaw6q</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Best way to paint nails close to cuticles</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aeaw6q/best_way_to_paint_nails_close_to_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ae9r48</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>These Russian Mani baddies</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae9r48</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ae9eeo</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Diy help</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae9eeo/diy_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ae9046</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>What do yall prefer and why? Acrylics or Gel X?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae9046/what_do_yall_prefer_and_why_acrylics_or_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ae8eue</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>I’ve been loving jelly on top of silver cat eye lately 💗</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufk317b7igfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ae8805</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Flexible nails? Help</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae8805</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ae7he6</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Acrylic vs polygel for press-ons. Which is best for cost and durability?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae7he6/acrylic_vs_polygel_for_pressons_which_is_best_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ae7b6d</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>pink romance</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxunmfs3agfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ae71cb</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>my first time getting gel x 🥰</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9fgxqq08gfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ae6um6</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Biab peeling after 2 week</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae6um6/biab_peeling_after_2_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ae6tyz</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Acrylic press ons</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae6tyz/acrylic_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ae68jx</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Do you like the freehand style?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aglu6b7a2gfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ae4wsf</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Non-Gel Velvet/Magnetic Polish Recommendations?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae4wsf/nongel_velvetmagnetic_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ae5sqr</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>How do I fix this?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw3s2al2zffc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ae5n8e</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Repost to remove a set with an expletive (sorry mods). Anyway Question is which nail shape works best!! (I included one in which I asked for a pride set and she chose atrociously 😂 they were corrected, most of my nail pics I lost)</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae5n8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ae5j0v</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Valentine’s is always my favourite theme 🥰</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0875bve2xffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ae5izs</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>apex/gel french tip question</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae5izs</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ae5fy1</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>My most recenttt♥️🫶🏻</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae5fy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ae4ecr</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Year of the dragon 🐉 my first attempt at a dragon 😅</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k0hdkw2uoffc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ae477u</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>My practice today, what do you think?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9v4508xmffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ae3off</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Pikachu Inspired</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pmhqb9ljffc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ae3hnq</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn9z59n8iffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ae37pz</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Ready for bright spring nails 🌸💐🌷</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ghndec7gffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ae2zr8</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Inspired by the beautiful red sets I've been seeing.</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn443enjeffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ae129d</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Where my press on peeps at?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jecinmt0ffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ae2g0t</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Fav glue on nails?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae2g0t/fav_glue_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ae0cml</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Tried Lily &amp; Fox nail wraps</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5b5tl0svefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ae2575</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Do I still have to buff/ remove shine from Apres Gel Tips before applying gel polish?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae2575/do_i_still_have_to_buff_remove_shine_from_apres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1adwyod</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>I have no idea what to call this design but I love it!</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jttbtzz56efc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ae1zj6</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae1zj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ae1v3v</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Is there any kind of “epoxy” material for nails? Think acrylic powder + monomer but liquid form?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae1v3v/is_there_any_kind_of_epoxy_material_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1adwb9c</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Nail Color for THE MOMENT!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1adwb9c/nail_color_for_the_moment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ae1m7i</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Painted trees!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae1m7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ae159y</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Is this normal for shellac?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5ut5xvf1ffc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1adrgar</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Why do I get these bubbles in my nails when they dry?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adrgar</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ae0w2o</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>3-4 months of nail growth</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ng2s5gzlzefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ae07z5</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Had acrylics removed at the salon/did dip mani myself at home</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae07z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ae0618</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Courage the cowardly dog!!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl7mahojuefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ae03ei</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Anyone that does cool nail art near Chicago?</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ae03ei/anyone_that_does_cool_nail_art_near_chicago/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ae029t</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Back to acrylic after a short stint of press ons. 😍</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0mxtiuutefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1adztbr</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>First and last time getting this shape🥲 .. can't wait to get back to my almonds.</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrswg4d2sefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1adzmx3</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Finally got into magnetic gel and I love it!</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eeiz717rqefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1adzcg2</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Simple &amp; Sparkly✨</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fg0lumtkoefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1adytcp</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>A dad on a mission - we tried chrome powder for the first time.</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adytcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1adxsqg</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>1 month of biotin supplements.</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7c0qm80scefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1adxjxp</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Did a cat eye set for the first time!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adxjxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1adxiz9</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>I love my work 🥹 what do you think?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adxiz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1adxgd2</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>would you consider this square or coffin?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvu2vp82aefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1adwazd</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>I had to get new nails for my upcoming trip to Belize!! 🪼</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfepbv5v0efc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1adw5p2</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Press on nails hazbin hotel</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3tytwsnzdfc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1adv6wr</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>You guys were right, there’s no going back now 🫣</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adv6wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1adttwi</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>My nails pink 🥰</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2telq6r9edfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1adtb8o</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>OPI You had me at Halo</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adtb8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1adsfea</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>My first time working with gold leaf 😊✨</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adsfea</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1adr68h</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Princess bubblegum nails!!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adr68h</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1aeiss1</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Witch craft!</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3e7sm2zz4jfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1aehg2k</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Oi, Prick?! by Swamp Gloss</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aehg2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1aehcty</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Bee’s knee’s lacquer “I have been crying out to you from the start”</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xiqi88baoifc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1aegvpa</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>This weeks manicure</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zpyqiybjifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1aegleh</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Color Club We’ll Never Be Royals 👑</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aegleh</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1aeg6ek</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Happy (late) birthday to me!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkr9xi98cifc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1aefv44</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Aqua Tofana by Dany Vianna</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/baccza169ifc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1aefrvn</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Molten Lava (again)</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24xjan5a8ifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1aefqy8</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Attempted wintry skittle turned out too seaglass-beachy so I covered it up</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aefqy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ae65qy</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Nail oil or clear coat</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ae65qy/nail_oil_or_clear_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1aef7do</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>ILNP Happy Hour</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aef7do</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1aeexv4</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>TMI: nail issues (gross) (sorry)</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aeexv4/tmi_nail_issues_gross_sorry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1aee25q</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Mooncat - Mercury's Tears</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aee25q</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1aedvpm</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>BKL buzz bags</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aedvpm/bkl_buzz_bags/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1aecmf5</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Oh my goodness I love this!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u27m57gcghfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1aec4gp</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Mooncat Moondust VS Holo Taco's Scattered Holo Taco</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aec4gp/mooncat_moondust_vs_holo_tacos_scattered_holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1aebnqb</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>who’s gonna be the first to showcase boolba?? 👀</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aebnqb/whos_gonna_be_the_first_to_showcase_boolba/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1aea6g4</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Rosary Pea Comparisons</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st7pw7mzvgfc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1aea1gu</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>January manicures :) ✨</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aea1gu</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ae9qpd</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>are polishes with hema okay for press-ons?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ae9qpd/are_polishes_with_hema_okay_for_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ae95w9</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Monthly Review Roundup!! (January nails, aka I’m in my Blue Period. Call me Picasso 💅🏻💙🦋)</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae95w9</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ae8fiv</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>It's not much, but it's honest work. 🩷💜</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w5fiyicigfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ae8890</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Mooncat- Which polishes are limited?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ae8890/mooncat_which_polishes_are_limited/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ae80t0</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Mulled wine 🍷</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vw0hdvbfgfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ae7zjx</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Spirit Fingers</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae7zjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ae7yqb</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Impressed by LynB</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae7yqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ae7u7k</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Can someone tell me what I'm doing wrong</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpiul7vzdgfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ae7eue</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Polish display and storage</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy4osxmvagfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ae7bv7</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Love this red so much I finished the bottle.</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae7bv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ae7a08</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Somehow I managed to overfill this drawer with just blues and purples...</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1k4wkuw9gfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ae77c1</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Cranky Frankie, 3 days of wear</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkjb4pca9gfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ae72kj</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Mooncat Millenia 💫</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae72kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ae6l4h</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Dreamy Nails 🌔✨☁️</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae6l4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ae6if7</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Famous Original</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okoe84sa4gfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ae6fqb</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Wildflower topper 🥀</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae6fqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ae6ae3</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>How many of you have tried Nailpollies?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ae6ae3/how_many_of_you_have_tried_nailpollies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ae5h9a</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Organising my polishes as I try and rebuild the collection</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pr1aj6pwffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ae4qbh</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Refreshed + SH Unicorn Top Coat</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2s9571q7rffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ae4juu</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Recs for a sparkly white shade with pink holo or glitter?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ae4juu/recs_for_a_sparkly_white_shade_with_pink_holo_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ae3st1</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Has anyone else experienced extreme top coat yellowing/darkening? I’m using Mooncat’s top coat</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae3st1</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ae3p6h</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>I can't control myself around pink to green shimmers</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae3p6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ae300q</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>mooncat obsession</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae300q</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ae2sux</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Same Lie Lilac - Bee’s Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3og6ad7dffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ae2e66</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Fav polishes you can get on Amazon?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ae2e66/fav_polishes_you_can_get_on_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1adw3dv</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Dragon's breath</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adw3dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ae1hl0</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Varicose Veins</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae1hl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ae1dzk</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Vampy V-day Red</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyyqli083ffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ae13t7</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>🔥 Hot and Cold ❄️</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ae13t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1adztu4</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>got my nails done for Chinese New Year. Should I be annoyed with the gold?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl2vmj16sefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1adzqv9</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>I love penguins 🐟🐧</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adzqv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1adznls</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Recent Copper Crackle Polish?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1adznls/recent_copper_crackle_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1adzlow</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>What top coat(s) and/or technique are you using to make your lacquer look like gel?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1adzlow/what_top_coats_andor_technique_are_you_using_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1adzkpk</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>A little 90’s grunge on an overcast day ☁️</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpn0x5laqefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1adzfrk</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Palate cleanser with a little added sparkle </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e5ld4s34pefc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1adzeqy</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Dupes for Mooncat Game Over?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwzgm7z1pefc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ady316</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>My favorite polish yet - Lavender Sky</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ady316</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1ady2ay</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Different vibes</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ady2ay</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1adxv2y</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Is it time for Valentine’s nails yet?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adxv2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1adx2r1</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Im a total beginner (male) looking for a way to get stronger nails for acoustic guitar fingerpicking and to prevent nail biting.</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1adx2r1/im_a_total_beginner_male_looking_for_a_way_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1adwbcm</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Next time I will have to coordinate my hobbies and have my manicure match my black king oysters during harvest. But for now, party nails!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adwbcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1advwaj</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Afterlife by Bow Nail Polish</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1advwaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1advno4</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Tried my hand at marble nails (don’t look at my cuticles)</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1advno4</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1advmd5</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Mooncat polish gloopy</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1advmd5/mooncat_polish_gloopy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1aduz3p</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>In love ❤️</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aduz3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1adtxej</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Feeling both fascinated and ambivalent about this one</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adtxej</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1adtnem</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Trying a new color for valentine's day</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adtnem</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1adtes1</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Essie's White Polishes</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1adtes1/essies_white_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1adsqbd</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1adsqbd/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ads0y8</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>What chrome powders do you guys like to use?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ads0y8/what_chrome_powders_do_you_guys_like_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1adrhan</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Gorgeous drugstore holo find 💚</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adrhan</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1adr5bi</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Y'all this is my DREAM nail polish (Enchantment by Fancy Gloss) but it's sold out. Does anyone have a dupe?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2ukpzvzicfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1aeh4bs</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>What could I search for to find more inspiration like these</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnyka7kulifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1aegig0</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Cherry Flavoured 🍒</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95vokycjfifc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1aeekr5</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeekr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1aebmeg</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Princess bubblegum nails!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aebmeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1aebk2v</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>My Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lscuwhpf7hfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1aeaszc</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>In LOVE with my valentines nails!!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeaszc</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ae5vrq</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Acrilics nails Barbie</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3ws0dfpzffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ae4snm</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Very proud of the C curve and overall shape on this sculpted hard gel set</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to80mqforffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1ae4lro</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Holo glitter galaxy nails ✨</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04dafrpcqffc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1adwi0t</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>me again = dark aesthetics again 👽⚔️</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxb6te9g2efc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1adshx7</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Gold leaf is pretty fiddly 😊✨</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1adshx7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan 31 08:07:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_04.xlsx
+++ b/data/2024_02_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C457"/>
+  <dimension ref="A1:C625"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8202,6 +8202,2862 @@
         </is>
       </c>
     </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1afctmf</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Need help buying a gift</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afctmf/need_help_buying_a_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1afc2wt</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>How do we feel about these?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sohlc32h7qfc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1afc0sc</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>I hate fake nails - how to maintain painted nails?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afc0sc/i_hate_fake_nails_how_to_maintain_painted_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1afbsnc</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Large-size nailforms?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afbsnc/largesize_nailforms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1afbdwx</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Started doing my own nails.</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afbdwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1afat71</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Thought I would share my nails 😊</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7e22eystpfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1afasjw</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>New Cherry Set</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ix2saultpfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1afa2bm</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Photos of the custom nails I designed with my nail artist! All hand painted</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afa2bm</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1afa1a2</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>In love with my nails!! Spent a while designing them with my nail artist, and she absolutely went off!! Everything is hand painted</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bv0ityt1mpfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1af9pg4</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Newest Mani</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yha3rtp0jpfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1af700l</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>hard gel done by me</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwtd7gxhuofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1af97va</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>I’m impatient. What can I use between coats to help polish dry quicker?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1af97va/im_impatient_what_can_i_use_between_coats_to_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1aexfju</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Tried glamnetic nails not impressed</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aexfju</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1aevdpc</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>How do I fix slight scuff in matte nail polish??</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o0ul67femfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1af8iyx</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Becoming slightly annoyed at my progress</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af8iyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1af8g0q</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>The Sandman Nails</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qil4t2c7pfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1af77h7</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>It’s starting to look a lot like Valentine’s Day ❤️❤️😘</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ilvrl22cwofc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1af4jdn</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>I want to make a nail set for my mom. How could she glue them on well?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1af4jdn/i_want_to_make_a_nail_set_for_my_mom_how_could/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1af68ll</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Blue 💙</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o94scqaunofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1af5u8u</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>2nd ever attempt at nail art; feedback and CC appreciated!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24g0lupikofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1af5ny7</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>valentine’s day nails💕❤️</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkwkigb1jofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1af5adv</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Nail polish recommendations for two different skin tones to coordinate/match?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcqeinbxfofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1af59ov</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>New Valentine’s Set</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv9j72prfofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1af4k9y</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Is there a regular polish dupe of this color?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fk7dil0z9ofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1af4evc</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Can’t tell if I’m being pickyyy or should I have said something</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af4evc</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1af4bsy</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Simple Red! 💅🏻</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muihokm18ofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1af468e</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Serving frosty queen</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af468e</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1af44zx</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Rate my nails :p (black with a glitter coat &amp; top coat)</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z49bqsvg6ofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1af3off</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Help with nail growth</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af3off</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1af3ig1</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Gave myself a manicure and pedicure today! 💅🏼🦶🏼</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af3ig1</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1af3cnk</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Obsessed with the Marbling 😍</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ju2nh4nc0ofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1af35w2</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Are there actually any good nail polish pens?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1af35w2/are_there_actually_any_good_nail_polish_pens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1af35o4</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>vday nails with magnetic gel !</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vviwci1vynfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1af1xn3</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>New color!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af1xn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1af1wbv</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Nude baby pink +bonus dog in the background</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6yzx6dapnfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1aezeyf</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>How to get past nail shape envy if you can't wear long nails?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cw7fyn5g7nfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1af10dn</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Which Valentine’s set di you guys prefer?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af10dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1af0dis</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Enchanted 🌹</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3zz39bbenfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1af08fn</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Low key obsessed with my Vday nails ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af08fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1af04i2</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>What color of chrome would I need to achieve this look?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9e4x6cjcnfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1aezu36</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Looking for a deep red.. but less goth.. but also not bright in sunlight</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szxal9shanfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1aezp37</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>V-Day Set</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aezp37</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1aezbte</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Blue cat eye nails 🩵 Reminds me of space</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/usoq8dps6nfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1aez5l8</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Valentine Nails 💅🏻 💕💘</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aez5l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1aeyv3i</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Last winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeyv3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1aeyp8i</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>🥺 best nail shape?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeyp8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1aey98o</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>This color combination will always have my 🖤</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ta9t030zmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1aey6ds</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Nail newbie: do I need to get a new set or will they shorten my nails during my fill?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aey6ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1aextg0</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>How do we all feel about glitter polish?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aextg0/how_do_we_all_feel_about_glitter_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1aex9k6</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>I like my nails how I like my wine, red 🍷</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixv0fc3rrmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1aewe89</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Just soaked the paint off and my nails are stained blue. Is this just a symptom of cheap paint, or can i prevent this?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5gbpwtilmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1aewby9</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>men's semi-permanent manicure</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4u7w2a3lmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1aevyoi</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Starting to really get the hang of GELX!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8f0tg4iimfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1aevstp</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Cookie Monster for a cookie addict</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aevstp</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1aevpo6</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>V day nails!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aevpo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1aevieo</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>did my nails for vday!💕</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v912k5ubfmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1aev7vx</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Do you think this is nice enough for my 5th year anniversary?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bchks9kadmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1aeuwl6</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Nail day</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeuwl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1aeuvm4</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>made them today 👽</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeuvm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1aeru83</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>How do you find nail polish colors that look good on your skin tone?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aeru83/how_do_you_find_nail_polish_colors_that_look_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1aergms</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Chip/Indents?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ursdsy5mlfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1aer5f8</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>First time black</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aer5f8</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1aeq5t2</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Looking for London based nail artist - and opinions on undernail skin growth please</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aeq5t2/looking_for_london_based_nail_artist_and_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1aetzpt</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>A less traditional Valentines set💜</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yt30q8f4mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1aetxve</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>My first attempt at tweed nails</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wy0xdxk14mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1aetxvb</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>what do you think of this</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqy7mco14mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1aetxt5</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Salon Press on Nail Application</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aetxt5/salon_press_on_nail_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1aetwul</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>did it on a hurry. i think it worked pretty well</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjo14a3u3mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1aetvpy</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>did my nails yesterday what do you think?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mbw9fjl3mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1aetupp</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>finally worked cuticules out with soft gel</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntn8jlde3mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1aetu0q</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>what do you think of this combination of colors</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i06z6zi93mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1aetpv4</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>baldur’s gate 3 nails on me by me :)</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aetpv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1aesx9w</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Nail artist wage</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aesx9w/nail_artist_wage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1aeso7z</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Show us your Valentine’s Day nails!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceapgrj2vlfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1aesfa0</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Just finished</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qox4eo0btlfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1aerzaw</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Love pedi set</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aerzaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1aern1x</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Do these look more brown than black?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aern1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1aer9t0</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Do you like these gel X extensions nails? Salon done.</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jqpodkqklfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1aer0uu</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Valentines Dip</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aer0uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1aeqo20</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Nail care steps</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aeqo20/nail_care_steps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1aeqh9p</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails 🩷❤️</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qk0tv2nnelfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1aeqc49</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>I ❤️ my nail tech</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6be7wjeldlfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1aepnpv</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>All the polishes and polish combos I’ve worn over the month of January 2024!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lr2p7n6y7lfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1aepemr</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Just got this yesterday…classy nails type of gal.</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnbhjhlr5lfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1aepapi</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Are these coffin or ballerina shaped?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bxh98uv4lfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1aep3m7</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>New nails.. again 😇</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyhutxl93lfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1aeof34</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>My new nails!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeof34</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1aeo8q2</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Pink chrome 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i8dnpiuvkfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1aensmo</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Transition from covergel to natural nails (help needed)</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aensmo/transition_from_covergel_to_natural_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1aenpnn</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Does this color remind you of wine? 🍷</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9exps1pyqkfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1aemy1w</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Had some fun with abstract lines!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmonw3n8jkfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1aemipe</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Black with Periwinkle tips</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6xx8t9pekfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1aelese</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Can you handle rhinestone of this size on your nails?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aelese</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1aekt7m</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>New nails, my latest work, experimenting with design I used white varnish, then I put a piece of cinder film on it, dried it in a lamp and put a pink base on top, I also sawed it out with a milling cutter and covered it with a top coat.What do you think?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mxhc19xtjfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1aekcbp</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>I’ve been practicing French tip nails</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymnuekxbojfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1aejhqa</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>#valentinesday #coffin</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wikqkqldjfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1afckq7</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>✨Lilac has me in a chokehold✨</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pehhv5sbdqfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1afchor</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Influencer discount codes?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1afchor/influencer_discount_codes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1afbckh</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Rainbow skittle 💖</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqoiocuezpfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1afayi0</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Together until the end - Phoenix</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afayi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1afauhy</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Swatches of the newer lechat mood polishes</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1afauhy/swatches_of_the_newer_lechat_mood_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1afah8d</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Late night mani</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/216lkusdqpfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1afaanr</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Is there a way to add thickness or an apex with just nail lacquer?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1afaanr/is_there_a_way_to_add_thickness_or_an_apex_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1afa7w2</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>I Can't Take My Eyes Away...</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afa7w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1af9md3</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Please tell me I’m not crazy</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af9md3</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1af24wd</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>IlNP "Enchantment"</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zo1hhc0rnfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1af8yhw</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>A fallen soldier 🫡</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmmgoutvbpfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1af8eia</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Birthday Nails ft. Coronation</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af8eia</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1af8bzt</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Has anyone dealt with this before?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af8bzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1af89ww</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Why did crackle toppers ever go out of style? I am living</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af89ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1af7uf1</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>New Favorite Red!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1af7uf1/new_favorite_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1af6lal</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>So… how many photos do y’all take of your nails?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0df4kvdwqofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1af6dlv</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>After two years of use, I find out these are touch screen compatible 🙄</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31cy68l1pofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1af6c25</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>I offered to paint my partner's (30f) nails</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af6c25</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1af60wk</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>When you’re a polish-aholic but you also have a job interview</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g2jxok2mofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1af5xp1</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Who cares about perfection? Send some unflattering pictrures of your current mani</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3joecjqblofc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1af5p2j</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>A magnetic finally worked!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7haq9m5bjofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1af5a85</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Game over - mooncat 🩷</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5ml2m0wfofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1af52q0</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>January Manis Part 1</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af52q0</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1af4j2u</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Is there a regular polish dupe of this color?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/alauqzxo9ofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1af4acv</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Those who use glass files: how long do they last for you?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1af4acv/those_who_use_glass_files_how_long_do_they_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1af3prm</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>INLP Overcoat</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af3prm</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1af2g04</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1af2g04/lurid_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1af1xjm</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Bee’s Knees - Chaos ✨</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jm9vg0jpnfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1af1hup</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>I didn’t love my mani so I refreshed it with new nail mail! 🩵🪩</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af1hup</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1af1bh5</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat x Holo Taco comparison (PR) </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/et9uq9l1lnfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1af07z6</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>First Time Using Kiara Sky Gelly Tips - Question</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1af07z6/first_time_using_kiara_sky_gelly_tips_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1af06oj</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>It's been a while since I attempted a nail art</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyax1r2zcnfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1aezjvr</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>New nail polish 💅🏿</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aezjvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1aeyva3</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>regular polish over gel manicure</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aeyva3/regular_polish_over_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1aeyouc</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>ILNP Shadow Grove</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeyouc</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1aeyn7r</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Mixing base coats?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aeyn7r/mixing_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1aewfh8</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Cock a Doodle Doom!</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9p7kfprlmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1aevqdr</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>LynBDesigns-Wooly</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8i35iougmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1aevjhn</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>A gorgeous drugstore find - it’s hard to capture on camera</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aevjhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1aevao4</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>First time I've done nails, anyway to prevent chipping in the back? Used Base coat and top coat</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8fz5mhtdmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1aev306</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Polished for Days Angel Wings</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aev306</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1aep9zm</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>My 1st Night Owl Lacquer</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aep9zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1aeu1hx</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Can anyone show me what ILNP's Hi-score looks like next to Holo Tacos Resting witch face (and maybe Party of one purple)?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aeu1hx/can_anyone_show_me_what_ilnps_hiscore_looks_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1aesmde</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>House of Hades</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aesmde</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1aes8ly</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Janny Manis</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aes8ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1aeryv0</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Drunk Fairy Polish “Flaminglow”</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeryv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1aerkww</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>ILNP Aspen is dreamy &amp; perfect for Winter!</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/px74to72nlfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1aerfh1</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Help me find a medium red creme somewhere between my favorite bright red and burgundy</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d8m1bzxllfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1aere9m</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Good light waiting for the subway</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ayhtk3cnllfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1aeqzpt</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Sheer Shifties ft Fairy Dust versus EdM Directions to Whereabouts</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeqzpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1aeqph7</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>H&amp;M - Peppermint 🍃</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeqph7</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1aeq3z1</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Shimmer top coat?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aeq3z1/shimmer_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1aepoy0</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>All the polishes and polish combos I’ve worn over the month of January 2024!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aahnx5998lfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1aepmi7</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Thundercloud under January skies</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1u8i036o7lfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1aeo1n2</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Not all magnetic are created equal.</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeo1n2</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1aenqri</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>recs for affordable and good-quality top coats available in India please. thank you!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aenqri/recs_for_affordable_and_goodquality_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1aenh55</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>ABCs of polish! N is for Noodles nail polish!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0nwwhklokfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1aendag</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Deciding between Holo Taco, Cirque, Mooncat &amp; ILNP for mega-order</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aendag/deciding_between_holo_taco_cirque_mooncat_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1aen7id</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Nails from the past month ft. some new favorites</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aen7id</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1aemso6</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>I broke a nail so I had to redo them. The theme is “dreamy”</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2b6z99wphkfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1aelhlf</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Love the clear rhinestone!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aelhlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1af93hh</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>emerald coffin set by me 🪩</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af93hh</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1af5wgc</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Press ons by me 😊</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ho3tpp1lofc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1aex2qz</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Hazbin Hotel inspired Nails ( Charlie X Vaggie Valentine's Nails) tutorial on my tiktok ✨</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dxk8q8cdqmfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1aew2s1</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Tell me what you think of my work</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qrix1zajmfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1aeuzx6</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>What do you think about my work? 👽</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeuzx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1aetvpk</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy2v2jcl3mfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1aesoi2</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>House of Hades</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aesoi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1aes7qm</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>My first press on application and design</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aes7qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1aerygm</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Love pedi set</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aerygm</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1aeqht2</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails 🩷❤️</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ym3cbtrelfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1aeldhj</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>I love big gem &lt;3</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aeldhj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb  1 08:07:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_04.xlsx
+++ b/data/2024_02_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C625"/>
+  <dimension ref="A1:C804"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11058,6 +11058,3049 @@
         </is>
       </c>
     </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ag5isk</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Nice cherry red 🍒</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4e9e442gxfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1ag5g52</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Long nails are getting in the way of my gaming...er, I mean typing at work!🤣</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yxxqty5fxfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ag4tzw</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>First Magnetics</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9cxrodm7xfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ag45t4</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Look at that cuticle clean-up🥵 My nails were in some need of TLC</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbk5ory10xfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1ag3dgz</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>IceGel Chrome powders have me in a chokehold 🤩🦄</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag3dgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1ag36t9</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>It is a very beautiful and perfect color.</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07yui3w4qwfc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ag2plg</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Funny bunny with a mini black heart 🤍</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3tvpioilwfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ag2de1</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Early spring nails I got done recently</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq796xx8iwfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ag2cwz</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>beginner nails on a budget 🥲</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs93x1m4iwfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ag1t4n</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Looking to sell my stamping plates</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ag1t4n/looking_to_sell_my_stamping_plates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ag1gct</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>It's the first time I use this color 😶</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ze3c8hzq9wfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ag1954</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Opinions ?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag1954</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ag0w0e</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Red and gold (and pink) for the new year!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag0w0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ag0qm8</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Nail glue that has a solution that makes it easy to remove without damaging your real nails?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ag0qm8/nail_glue_that_has_a_solution_that_makes_it_easy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1afyzl7</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>lisa frank inspo</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afyzl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1afyvgk</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>How hard is it to learn how to use builder gel?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afyvgk/how_hard_is_it_to_learn_how_to_use_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ag0nku</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>(Pic from @nailziana on IG) Best pink to dupe this!?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1ndxsjn2wfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ag0hop</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Valentine’s day nails 💌💋</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag0hop</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ag0byc</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Couldn’t wait any longer to do some v day nails!</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag0byc</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ag0b4b</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Look! Today I had my nails done, do u like it?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag0b4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ag00eu</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Tiny hearts</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag00eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1afzl64</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Valentines 2024</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2jsw9oftvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1afzfjt</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>January Nails 💙🥶 (yes these last all month)</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8l34h45svfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1afzd5s</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Slowly getting used to nail art</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9iwbsujrvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1afyweg</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>thought y’all might like my nails !</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5ho5jpinvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1afyuj9</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>💕</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xnj2s603nvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1afymjh</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Any brand recommendations for someone trying to diy gel?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afymjh/any_brand_recommendations_for_someone_trying_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1afyi1f</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails 💗</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqj48z05kvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1afxg86</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Question about a thick top coat on my thumb.</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afxg86</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1afx43s</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Valentine Nails - Dark/Rose Inspo</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6w1u4ckm8vfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1afworr</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Bacteria and fungi inspired nails 🍄</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3mcqj8c5vfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1afvf4d</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Why won't my acrylic harden?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqzhqu9svufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1afy3m6</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Pay by the hour as a Manicurist in Los Angeles ?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afy3m6/pay_by_the_hour_as_a_manicurist_in_los_angeles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1afxqy5</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Regular Sally Hansen polish on natural nails. Early Valentine's edition</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmhfknsudvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1afxpqn</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>got my first ever set!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afxpqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1afxhty</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Been practicing making my own gel...</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afxhty</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1afxbxm</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Anybody know a match for this color of nail polish?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buvgvi5favfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1afvzyt</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>One of my favs</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zwsep730vfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1afvg15</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>I’ve been really enjoying sparkly noods w chrome</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5678vuxyvufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1afv5ul</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>early Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afv5ul</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1afuk1n</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Feeling blue?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6yae30dpufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1afuir2</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>5 shades of blue tips</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gikarna4pufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1afu3kz</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>💅</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afu3kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1afu1oe</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Is this normal? Why do most at home techs require to come with bare nails?</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afu1oe/is_this_normal_why_do_most_at_home_techs_require/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1afts39</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Dainty lil floral frenchies</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afts39</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1aft1w0</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>My first time isolating chrome over a design 🍒❤️✨</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jjz4dtgeufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1afsaxt</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>What type of manicure will get me the thickest nail?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afsaxt/what_type_of_manicure_will_get_me_the_thickest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1afs6cr</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Crazy cat lady casual</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8iioljr58ufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1afq99v</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>why do my acrylics get scuffed up every single time?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afq99v</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1afpcd4</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>How to take care of gel nails?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6yrtwjuntfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1afsx8a</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Valentine's DIY set 💗</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afsx8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1afsu4y</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>I'm not getting married but I still love the bridal vibes 😄</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbo732xwcufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1afsmb3</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Gel X Questions</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7f4i0acbufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1afsego</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>First gel x set, does not look right.</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afsego</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1af9you</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>How to remove press on nails without this happening?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1af9you</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1afrpra</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Already did my “once a year” pink nails for 2024 😅💕</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afrpra</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1afrn1e</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set #1 🥰</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afrn1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1afrenr</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Gel polish peeling off of BIAB</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afrenr/gel_polish_peeling_off_of_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1afrce8</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>this black is perfect!!!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuhqcg272ufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1afrb9z</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Polishes that match these colors?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mb0hf5cz1ufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1afr6b1</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Valentine’s Day pink and red❤️</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq0u23dz0ufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1afqw9i</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Hearts are my Favorite ❤️</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afqw9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1afpo1i</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>First time doing nail art, any tips for improvement?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afpo1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1afphlh</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>first time nails</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afphlh/first_time_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1afp7b3</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat Eye Color shifting fun from the fall </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aa9bn10tmtfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1afovpl</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Structured manicure done with hard gel on my client’s natural nails ♥️</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afovpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1afoccd</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>💅🏻💅🏻💅🏻</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01w26rimgtfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1afnkdz</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Ready for valentines 🥰</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nstgml4btfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1afnguy</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Spirited away! Ahhh I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn8arjqeatfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1afna7a</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Do I pull it off well? Glass nails, my first gelx attempt 💎 ʚ(* ´꒳` *)ɞ 💗✨</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj8zef739tfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1afmyt7</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Need help! Should I add something more?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afmyt7</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1afmupb</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Question about OPI Start to Finish 3 in 1</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1afmupb/question_about_opi_start_to_finish_3_in_1/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1afmjir</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Went for baby pink natural nails 🐹🌸🍓</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nziv6s5t3tfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1afmgjv</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Boho Mermaid Acrylic</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngofmbo63tfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1aflzif</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aflzif/new_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1afljed</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Fabulous chrome!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afljed</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1aflfqy</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>cherry croquette frenchies for february 🍒💌🎀</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aflfqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1afl8w2</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nails</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afl8w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1afkfbu</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Marble nails 🥰</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8d1d2wpnsfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1afkarp</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Simple black with a touch of Cateye</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kiy79l1pmsfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1afk3rn</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>🫦🥀</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afk3rn</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1afj0x0</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Jelly red &amp; silver cat eye 🩸</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2kqnojvgcsfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1afim4o</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Not stylish…</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65say3fx8sfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1afhuj7</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>There’s a first for everything</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdecn61d2sfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1afgulu</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Been doing my own</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pco4i64ssrfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1afgol7</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>My first time painting flames🔥</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afgol7</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1afgd12</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Valentine Nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm0nicwpnrfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1afgc7u</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Why is cuticle skin so ragged?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afgc7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1afft40</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Ombré with stars</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afft40</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1afenqj</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Does this nailshape fit me?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afenqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1afen1c</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>I tried 😭</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tca3jjg3rfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1afdz0v</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Cannot go wrong with red!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afdz0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1afdxqx</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>My nail art work.</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ropgo96fuqfc1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1ag582l</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Help me pick out my valentine's day nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag582l</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1ag4yk4</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Bees knee’s lacquer fair winter lady</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/umm8nhw59xfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1ag2kva</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Dupe for OPI mod about you (pastel version)</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag2kva</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1ag4utc</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Oh the irony....</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyituzmw7xfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1ag4mfu</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Mooncat-Sand Viper</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jucfwg705xfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1ag4f8k</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>How much do you guys spend on nail colors per year?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ag4f8k/how_much_do_you_guys_spend_on_nail_colors_per_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1ag3zlr</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>First Time with Zoya..</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ag3zlr/first_time_with_zoya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1ag3ov2</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>How to save a breaking nail without doing a teabag patch?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ag3ov2/how_to_save_a_breaking_nail_without_doing_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1ag3egu</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Why yes, I did get a custom polish inspired by my cat</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag3egu</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1ag2tfe</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Nail art attempt - flowers</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag2tfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1ag1wsl</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>ORLY - Wistful Water Lily</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag1wsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1ag0y9a</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Went for a geode look</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg3wh6r85wfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1ag0y75</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Help me pick a nail shape!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag0y75</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1ag0lsp</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Making Boolba work 🤞</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fcuosp62wfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1ag031x</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Surprised by Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0ls56fpxvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1ag0122</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>January Manis Part 2</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag0122</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1afzpal</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust never disappoints</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afzpal</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1afv3gn</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Loving this thermal!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afv3gn</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1afxykk</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>6th Station is best in grocery lighting</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07i94f4mfvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1afxnlh</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Mkay!</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6eexb393dvfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1afxmge</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Ghastly Smell- Psyche Minerals my birthday manicure! Holy sparkles batman! 💕💕✨✨</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/83rnxjpscvfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1afxf7d</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Colors of January</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afxf7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1afwn63</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o95ji9905vfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1afwk5l</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Sign #402 you've been scrolling this sub too much: Taking awkward holding things pics</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afwk5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1afvth2</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Should I make them matte?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afvth2</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1afvmt1</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Finally, a seasonal chance to wear all the colors I don’t normally grab for my day to day!</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afvmt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1aftexg</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>A lovely shade for a wedding this past weekend 🩷💐 Polishes Used: Zoya (Shade: Patrice) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aftexg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1aft90p</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Didn’t get the best pics but this is a nice dark green 💚 Polishes Used: Nail Hoot (Shade: Turaco Me Crazy) | Sally Hansen Miracle Gel (Shade: Moonlit Top Coat) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aft90p</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1aftqnq</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>A juicy skittle 🍓🍒🍐🍏🍊</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aftqnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1aftmv5</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Sometimes you just need a little holo sparkle</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aftmv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1aftg8o</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Green on green on green</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4gtvezbhufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1afskxb</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Frosty ❄️</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afskxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1afs9yt</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>First day of No blue/purple February...</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afs9yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1afs0lt</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Any polishes similar to Phoenix's Rainbow Fluorite or I'm a Nerd?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1afs0lt/any_polishes_similar_to_phoenixs_rainbow_fluorite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1afrtd5</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Garden Path, Sweet and Sour, Drunk Fairy, BKL, and Phoenix</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afrtd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1afqw9u</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>boolba …</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afqw9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1afqv03</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Trying to convince myself I like this one. My matching friend here helps!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dycrs03sytfc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1afqnir</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Polishes that match these colors?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imx2082axtfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1afqfac</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Orly Ma Cherie</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09jrn1rkvtfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1afpem1</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Azalea Bloom by Beaux Reves</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afpem1</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1afoxst</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Paradox Polish - Wisteria</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afoxst</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1aforod</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Simple blush/nude sparkle mani!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aforod</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1afnr2l</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Dupe for polish</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzfh52mfctfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1afmtn1</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Rosary Pea is gorgeous, but wear a base coat!</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afmtn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1afmjl2</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Celestial Skittle 🌜✨🌌</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afmjl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1afmhd3</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Springtime Shorties 🌱</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afmhd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1afmel8</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Seen on Instagram - how would I describe this shape and length to a nail tech?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afmel8</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1afmdw3</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>I like how these turned out</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3fooxtn2tfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1afm6o7</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>My OPI Plumping top coat is getting thick and gloopy. If I add thinner, will I lose the plumping effect?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1afm6o7/my_opi_plumping_top_coat_is_getting_thick_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1aflzgj</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>how long (on average) does it take you to do a new mani from start to finish?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aflzgj/how_long_on_average_does_it_take_you_to_do_a_new/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1aflrdj</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>This is beautiful, but…</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aflrdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1aflnsf</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>The longest I've ever gotten them! (already broke and trimmed down tho)</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytt630zpwsfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1aflfti</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>I've had bad luck with Essie but finally found a color by them that I love! Lilacism</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aflfti</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1aflf2t</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Bill Round 2</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aflf2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1afl7o3</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>I don't do oranges often...</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2ep3w2vtsfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1afktkc</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>What are your favorite neutral jellies?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1afktkc/what_are_your_favorite_neutral_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1afkd3n</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>My birthday nails!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afkd3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1afk7x8</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>A little pink-me-up for a bad week</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kn7l4g4msfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1afjwsr</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Pleasant surprise with this thermal!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/EQoQhHK</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1afiqfj</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>White Night / Riveting 🤍🧡</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afiqfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1afimbn</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>{PR} My red 🥰</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afimbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1afhyyf</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Rosary Pea ❤️</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afhyyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1afhwa2</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>It's a lot more glowy in person</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afhwa2</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1afhh3p</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Essie polish never seems to dry</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1afhh3p/essie_polish_never_seems_to_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1afhegx</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>You could say I’m a MILF</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afhegx</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1afglfi</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Yesterday's flea market find</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0y6t7o5qrfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1afggd3</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>How to disguise my very solid white tips?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c21gh8porfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1afe0w5</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Christmas X Valentine!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afe0w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1afdbuc</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Cock_a_doodle_Doom - Application &amp; Different Lighting</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zyfjoe7fmqfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1afdaqw</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>January Manicures!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afdaqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1ag1zwu</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Aura nails</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag1zwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1ag1f5x</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Press on Sets</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag1f5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1aful7o</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Simple and sweet ☺️</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsvc31alpufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1aftr71</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Dainty lil floral frenchies</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aftr71</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1aft5ou</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>My first time isolating chrome over a design 🍒❤️✨</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnv8ic87fufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1afrbi2</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>how deep is this black 🤯</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gincgbm02ufc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1afqf9c</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Soft blush nails 🎀</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afqf9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1afoieo</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Nail art by me 💕</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zzg860vhtfc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1afmg2e</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Boho Mermaid Acrylic</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmo99j833tfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1afly54</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Today I made this design by hand. how about?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afly54</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1afjx36</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>How do I get this nail stripe tape to stay down?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afjx36</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1afixq5</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>This one was "maximum effort" :p</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk1xmkzqbsfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1afibpg</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Nail</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8shldh0j6sfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1afgl7e</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>My first time doing flames 🔥</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afgl7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1afdx1k</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>My nail art work.</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvaf14x5uqfc1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1afdwxc</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Red is such a magical colour!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1afdwxc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb  2 08:07:44 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_04.xlsx
+++ b/data/2024_02_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C804"/>
+  <dimension ref="A1:C935"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14101,6 +14101,2233 @@
         </is>
       </c>
     </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1agy89b</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>my valentine's set</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iio1xa6tk4gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1agxy0f</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Nail Decals / Stickers</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agxy0f/nail_decals_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1agxnrs</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Nails for Wear Red Day for heart disease awareness</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agxnrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1agwoch</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>It’s giving fairy core!</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agwoch</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1agr9rx</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>what I got (@nailsbysandyyy) vs the inspiration (@sydney3threenails)</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agr9rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1agllxe</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Nails damaged from polish</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fujlsglhg1gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1agky91</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>It can take me 8-10 hours to do a basic gel set 😕</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agky91/it_can_take_me_810_hours_to_do_a_basic_gel_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1agw2xi</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>🪲🐞 lil bugs 🪲🐞</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agw2xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1agupc1</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Y2k design requested by my client!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agupc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1aguisf</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>First set of nail art I’ve done.</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aguisf</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1agtb5j</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>(Beginner) Galaxy Nails 🌠🪐💅🏻</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urpz0le063gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1agsb1f</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>did these last night 🩷🍓</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agsb1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1ags1pd</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Base coat is base coat, right?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ags1pd/base_coat_is_base_coat_right/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1agrgec</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>I’m single but made these for my sister’s valentine plans 👀🎀</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agrgec</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1agr84q</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Pink Frenchie</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qksojfszn2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1agr4bg</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>magnetic cat eye gel is my new favorite thing 😻✨</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aa4pfie3n2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1agqxl6</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Choosing 10 colours for one hand was difficult 🤣</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhqd66vil2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1agqahe</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>conspiracy?!?!?!?!</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agqahe/conspiracy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1agq49a</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>She's bright</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k618qajte2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1agpohw</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Nail care as a baker by profession?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agpohw/nail_care_as_a_baker_by_profession/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1agp5rg</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn7gff3b72gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1agoch8</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>My first time trying builder gel 🥰</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywzynps212gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1agnwol</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>One month of OPI Nail Envy</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu7krjtsx1gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1ago3sx</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails I did 💌</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ago3sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1agnrb0</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>It fits me?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwy8arzow1gc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1agmovz</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Ombré pink glitter heart nails ✨💕</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agmovz</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1aglt2k</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Type of gel/finish</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6q7gljt1i1gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1aglp7e</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Help on what nail tips to use for short press ons</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aglp7e/help_on_what_nail_tips_to_use_for_short_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1aglfcp</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Natural Nail Growth/Valentine’s Day Nails!</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aglfcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1agl53n</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Steel Blue chrome 🪩🩵</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klne1sz2d1gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1agkpj1</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>What is the best system for a gel x style at home kit?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agkpj1/what_is_the_best_system_for_a_gel_x_style_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1agkgux</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>My favorite press ons from nailbaeLA.com</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dilh5xt281gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1agiq7i</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>I love Valentine’s day</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agiq7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1agible</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>GelX attempt</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol6hv4a7s0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1agi4my</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>My valentines nails :) if they last that long anyways</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m07ehkbrq0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1aghinh</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>valentines nails !! (inspo by @mel.nailed.that on insta)</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aghinh</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1agh8n3</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>So simple so fresh so clean</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agh8n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1aggxt7</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Structured manicure done with hard gel on my client’s natural nails ♥️</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7e73jk2qh0gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1aggb8z</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>How do you scoop up the product from a small jar with long nails?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aggb8z/how_do_you_scoop_up_the_product_from_a_small_jar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1agfajb</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Any advice for a beginner?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4dsdill50gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1agez85</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>I got my nails done yesterday for my birthday! Inspo from u/ava_lee00 on Reddit</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agez85</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1agg5z9</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Nail options?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agg5z9/nail_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1agfzyu</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Happy February 1st🤍🎀✨</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agfzyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1agfvvw</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>First time painting my own nails with gel polish ⭐️</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agfvvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1agf2pd</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>DND Ferrari Red with BIAB 😍</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzepct3040gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1agf1lr</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Nails chipped after 1 day</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agf1lr/nails_chipped_after_1_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1agdv5q</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Deadly Valentine’s 🖤❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agdv5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1agcvy4</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>What color nails should I wear with this dress?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ulm36g03nzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1agcmml</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>"Going Vogue" by Gelish</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vwtsl4xkzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1agcjmw</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Just thought about posting my current set 😊</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofd4oyv7kzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1agbzvn</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>I love me a girly pink set! Especially in February. What color do you guys have this month?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69dbn4ntfzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1ag9khn</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Deep Field</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag9khn</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1ag77rp</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>My new set🖤</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag77rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ag6hke</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Polygel recommendations</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ag6hke/polygel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1ag6b2c</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>would poly gel be good for someone who works an active job?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ag6b2c/would_poly_gel_be_good_for_someone_who_works_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1agxoa1</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Long Lasting Polish/Fake Nails for Fragile Nails?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1agxoa1/long_lasting_polishfake_nails_for_fragile_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1agkb29</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>rainbow trout nails, shoutout to u/spicygambit / @lacqueredactyl for this combo!</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agkb29</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1agvfc0</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>What is with the new trend of starting nails/polish halfway down the nail??</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1agvfc0/what_is_with_the_new_trend_of_starting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1aguz4g</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Getting around to using my polishes from the Zoya sale</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cw1i73lnl3gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1aguwf6</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Client wants everything on her nails!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aguwf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1agtsh9</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Some simple nail art</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36d5c3kba3gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1agspj0</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Wanted to share my nails again!! I’ve been loving regular polish recently</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p94y10yo03gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1agsfu5</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>A thick coat of topcoat saves the day</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agsfu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ags6ne</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Adore</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rql2of8w2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1agrm1p</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Budget Overcast skittle</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agrm1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1agqm2x</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>A Deadly Remedy - Anchor and Heart</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agqm2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1agq8mu</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Spirulina</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agq8mu</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1agpkka</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Stained Glass Vibes</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ashhi0rja2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1agpk6b</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Are the pearls weird? Be honest...</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc25vb4ga2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1agp0mj</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Opi my favorite gal pal. First time wearing and I'm already bored with it 😭</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agp0mj</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ago308</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Where my Portugal. The Man fans at?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ago308</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1agnyw5</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Tragedy</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agnyw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1agn09f</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Why did I think velvet nails would be difficult?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9prydna3r1gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1agmrn5</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Cutting cuticles/nail fold</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1agmrn5/cutting_cuticlesnail_fold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1agmnzi</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Neutral pink jelly press on nails :)</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agmnzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1agmecw</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>ILNP Cutie Pop</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0arl6nyjm1gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1aglzeo</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>I love shimmers!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aglzeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1aglkr3</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Phoenix - I don’t know what Christmas is</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aglkr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1aglj4r</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>How’s the color?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aglj4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1aglfrd</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Subtle grey-dient</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9jzdco9f1gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1agknb0</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Am I using a glass nail file wrong or is it the quality of the file?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1agknb0/am_i_using_a_glass_nail_file_wrong_or_is_it_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1agkhhu</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings 🍏</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gks0a5y781gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1agk0fm</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Angel Wings - a glowy pink for February 💖</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agk0fm</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1agj42n</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>All of my January manis + My Opinions™</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agj42n</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1agihua</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>My favorite multichrome 🖤</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt6evw7gt0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1agih7x</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Essie expressie "skip the track"🪻</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6zs9ckbt0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1agig9u</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Vaporize</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agig9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1agia2q</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>New Years Resolution</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agia2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1agi0zd</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Starting off February with Ethereal Lacquer Queen of the Underworld</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmcvgpizp0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1aghs3e</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>🎀Bow-eutiful🎀</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aghs3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1aghp2h</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Not the best or cleanest, but I semi-figured out velveting AND nail art!!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aghp2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1aggwk1</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Essie Not a Phase</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aggwk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1aggsd1</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>has anyone tried this trick with non gel magnetics?</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb73dtnmg0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1aggqqn</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>New Orly Neons?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtvzw12ag0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1aggj5p</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>First time doing my own nails in years :))</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aggj5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1aggh6b</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Happy February 1st ❤️</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0p5oxrfbe0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1aggesn</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Sheer nude shade that's less pink and a little darker than OPI Bare My Soul</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfkjqb8ud0gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1agg6n8</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>New nail polish case/carrier? Not in this economy</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agg6n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1agftph</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Wholesome thermal goodness 🫶 (Alchemy Lacquers🪻Hydrangea🪻)</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uxmu13j90gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1agfr5t</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Barbie fingers are back</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7wphzm190gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1agfqzx</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Stinky nail polish 😬</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nve25i090gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1agexd0</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>A month of growth since starting to use OPI Repair Mode</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7rdmmhv20gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1agemyy</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>What are your favorite iridescent nail polishes?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1agemyy/what_are_your_favorite_iridescent_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ageetp</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>I like to find random things that match my nails</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1kvehvzyzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1age5ix</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Looking for a green to match my favourite jacket (available in the UK)</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyiw39i2xzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1agdwzj</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Sunken Splendor drying with bubbles/rough texture for anyone else?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agdwzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1agdw9i</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>i topped one PPU with another PPU and created a secret third PPU</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b2rq111vzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1agdeoj</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Baby hearts ❤️🥺</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agdeoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1agd8jx</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>M&amp;N duo: Poisonous and Wolfsbane Recast</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ydo238tspzfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1agd0yv</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Mooncat Velvet Rose</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m22nrjf5ozfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1agctso</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Recovering nailbiter</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7jsq4clmzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1agcqr4</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Mossy Mani</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxauovwvlzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1agcbca</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Adding to the Rosary Pea Manis</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4f881bcizfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1agbw9t</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Hopping on the Aspen train 🚂</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agbw9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1agbldt</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Had to cancel plans so I need to share my fresh mani so SOMEONE. Sees it...</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdd9rukjczfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1agbkf3</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>This colour reminds me of the ocean 🌊</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrr4ggjbczfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1agbdrs</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Everyone walk the dinosaur 🦖🦕</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou0364zpazfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1agaqng</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>aruba by essie</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aw7v8fyv4zfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1agao8e</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Honest opinions on how these look?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/caf6wvq84zfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ag9i63</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Deep Field</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ag9i63</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ag9b5z</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Recommendations please!</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ag9b5z/recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ag8gei</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ag8gei/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ag7caz</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Phoenix Guitar Solo🎸✨</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qsgp0ka13yfc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ag6lna</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Boolba</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s9u8fsetxfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1agulh3</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Y2k design with HUGE stone!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agulh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1agq7rm</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Hello Kitty Valentine's Day Inspired</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umx3rdzlf2gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1agei3u</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Be my Valentine 🖤</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apsq6znnzzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1agdmgv</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Anyone else addicted to red? My client Lorena always tries to make me that color</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agdmgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1agd7xe</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>French Nails</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2tu9ypnpzfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ag9ylv</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Memphis Art Inspired</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meglutzgxyfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ag6kp8</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>I really like metallic elements in manicures 👻</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ywv7qj2txfc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb  3 08:06:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_04.xlsx
+++ b/data/2024_02_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C935"/>
+  <dimension ref="A1:C1119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16328,6 +16328,3134 @@
         </is>
       </c>
     </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ahr1kl</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>New nail lady I give her an 7/10</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahr1kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ahqz3r</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets from the last few months 🥰</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahqz3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ahqyq4</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Growing out natural nails with acrylic.</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahqyq4/growing_out_natural_nails_with_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ahqmjk</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Are these different colors or am I tweaking</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahqmjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ahqagn</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>fresh gel-x mani</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nm89x4w7lbgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ahqap5</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>My Valentines Day Nails 💕</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m00p7ddclbgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ahpro9</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>pink nails w/ initial</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqv1sstafbgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ahp91w</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Why does this always happen to my Gel x?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rybrpph9bgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ahp90t</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>A set of nails I did up for a friend</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xgd7yi89bgc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ahp3rc</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Oh my gosh. YALL!!!!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlpvyiez7bgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ahourv</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Mani and Pedi Advie</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahourv/mani_and_pedi_advie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ahoue8</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>What do we think? ($75USD Hand drawn)</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahoue8</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ahn700</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Would it be weird to get nails done with one finger injury?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahn700/would_it_be_weird_to_get_nails_done_with_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ahmz96</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Press Ons by Me! (Inspo pic from Pintrest by The Nail Lounge Miramar)</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahmz96</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ahmfbo</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Everything I need to start acrylic nails at home</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahmfbo/everything_i_need_to_start_acrylic_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ahlt5v</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Sailor Moon inspired nails by Shauntelle Hubbard at Shear Mellegence salon in Radford, VA</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c57ytpfobagc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1aho626</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>FIRST TIME doing gel nails, give me all your tips and tricks please! ignore the wonky rhinestones, they were a last minute addition and I got frustrated lol.</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aho626</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ahn5bf</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>lil conversation hearts</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djc1uxgboagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ahmwi0</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Nail tips improving</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahmwi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ahmgdc</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>DIY dip powder and nail art - Valentines set 💌</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahmgdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ahlsy4</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>new nails 🎀</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahlsy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ahlsaz</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>The perfect pink</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahlsaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ahl4o0</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Kiss Glue on Classy Premium Fashion Nails</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahl4o0</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ahl2s7</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Kiss bare but better press ons</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahl2s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ahjipa</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Press On For Now</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahjipa</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ahj7an</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>💖</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5c3aah8o9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ahj2as</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>My Winter Nails ☃️</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahj2as</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ahj2ah</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>I think I hate them &lt;/3</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahj2ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ahj133</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Strawberry Nails🍓</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he5qjjfrm9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ahihaq</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Flameo, Hotman!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahihaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ahif8g</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>What A Pansy by China Glaze</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkpzkisoh9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ahif0j</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>My natural nails</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz68bffnh9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ahidyy</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Lunar new year set</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg6t1ofeh9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ahidt6</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Wanted to share my January nails before I get them done next week: Monopoly nails by @nailzdesignzc on IG</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6e6j9fdh9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ahhujf</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Dip powder on natural nails. Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rvrwej5d9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ahhhoi</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Precious moments set I did!</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jfoptsca9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ahgmrw</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Valentines set! Done by Corner Nail and Spa</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahgmrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ahg672</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Valentines by moi</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pgso8yb09gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ahg3k6</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Work nails</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahg3k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ahfyvp</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Worst OPI Gel Polish Coverage.</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6soe92dry8gc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ahfus2</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Advice with Polygel-Dual for Desings</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahfus2/advice_with_polygeldual_for_desings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ahfu9s</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>If you were going to create your dream wedding nails, what would they look like?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahfu9s/if_you_were_going_to_create_your_dream_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ahfero</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>how are my nails?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahfero</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1ahcn3w</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Did my own at home Après Gel-x for the first time and this is what my natural nails look like after removal. Is this a reasonable/expected level of damage?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb6qrrs598gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1aheqfg</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Floral set for Valentines Day!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w792swk9p8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ahcvc7</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Are they good?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahcvc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ahdrh5</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Advice please!</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2h23ol2i8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ahdk4a</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Birthday Nails (02/02)</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsrid7nig8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ahdgpk</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>First time ever doing gel-x nails</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoiqgamsf8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ahccf0</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>How often do you get your nails done?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahccf0/how_often_do_you_get_your_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ahcduf</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Nice warm day to get nails done</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5aa1luj78gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ahdddp</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>My simple valentines set 💌</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1es82go3f8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ahcw07</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Valentines</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahcw07</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ahcp7e</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Black History Month Nails</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ncfn7exx98gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ahcggx</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>gel polish pocket lifting</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahcggx/gel_polish_pocket_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ahc1b9</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>am i overreacting?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahc1b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ahbqm6</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Happy Lunar New Year 🧧🐉</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahbqm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ahbmd1</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I just learned about this sub! I love getting my nails done and never have anyone to show them to. I got these done for valentines day. Short, round, and simple 🩷</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2gdc5sn18gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ahbetj</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Flat nail beds - nail envy + gel?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ahbetj/flat_nail_beds_nail_envy_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ahar3n</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Press on nails for February</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/454gi047v7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ahail1</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Cowboy Boots 🤠</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahail1</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ahaawt</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Ready for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzqrvetpr7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ah9vxb</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Nail drill questions</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ah9vxb/nail_drill_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1aha39o</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>got charms for the first time !!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aha39o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1aha2r8</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>♥️♥️</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd8qo2a1q7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ah8xr8</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Help with overfiled nails</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ah8xr8/help_with_overfiled_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ah89i3</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Dragon’s egg nails</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/64ox6g1gc7gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ah6jfm</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>What should I get tomorrow?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5v0skibz6gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ah5zai</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>How do I fix my nails?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rcek23tu6gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ah8xkz</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>I love my nail artist i swear</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u10n1nkfh7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ah8n9i</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Golden Tips!</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k1o2p7af7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1ah8rm2</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>i’m planning on getting acrylic nails for the first time soon, what should i expect/how does the process work?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ah8rm2/im_planning_on_getting_acrylic_nails_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1ah8pwq</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Valentine's nails!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5oeald0uf7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1ah8n5q</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>My first successful set I did on myself! :)</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f9hpof0f7gc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ah89wl</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>can’t remember the last time i got a design, and they turned out so cute!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5fnxy9kc7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ah7vem</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7omo3pj97gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1ah7pnu</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>first time having my nails done and i feel like a princess</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq7erurd87gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ah6ku1</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Too light of shade?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah6ku1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ah6k9m</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Snake Nails</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7qdsgjiz6gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ah6eb3</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ah6eb3/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ah4ry2</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Reliving my mid-2000s glory days</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah4ry2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ah30xw</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Top coat decision?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah30xw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ah1xxd</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>My valentine’s nails!</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uuhrtx4v5gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ah1vsv</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>All you need is love ❤️</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cpkf2ohu5gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ah1v72</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>OPI Nail Envy new formula</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ah1v72/opi_nail_envy_new_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ah0me8</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>My new Valentines set</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esfjd29nf5gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1agzl4z</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Loving these!!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agzl4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1agz9f7</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Rubber base for beginners</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1agz9f7/rubber_base_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1agz8l9</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Some Pink</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agz8l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1agyz34</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Done my own nails</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agyz34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1agytt7</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Love month design</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9qgwl5es4gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1agyrvb</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>My first set I did myself! :)</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1agyrvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1ahqirw</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Travelling to the USA from Canada, any places to hit to buy nail polish?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahqirw/travelling_to_the_usa_from_canada_any_places_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1ahpimd</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>I'm in love!! Kelp Kingdom</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfkudc0hcbgc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1ahpdgr</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Cuticula qdtc ruined my mani</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahpdgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ahoggw</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>It Really is Just Beautiful 😍</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpk1jcf91bgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1aho8wr</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Barbie legs… but make them nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkk4ukq4zagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1ahny2n</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Love these colors together!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shoyjcu4wagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1ahnrl4</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>January Wrap Up + Review</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahnrl4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ahnevg</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>New shelf</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7cgfqmwqagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ahn7p2</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Set</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/538kybdzoagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ahn7be</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>One week of a Hayride</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cga2vtxuoagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ahmvun</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>If you were starting from scratch, which products (base, topcoat, tools, etc) would you recommend for the longest lasting manicures?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahmvun/if_you_were_starting_from_scratch_which_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ahmq4y</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Some more fairy dust for your feed 💖</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sck769sakagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ahmh2y</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Mooncat Supervillian</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahmh2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ahm0bl</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Galentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahm0bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ahlswk</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Is it too early for Valentine’s Day nails?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/graim8wlbagc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1ahlhvi</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Gluing on nails painted with gel polish?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahlhvi/gluing_on_nails_painted_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ahlfmr</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>I’m about to give up on magnetics 😭</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahlfmr/im_about_to_give_up_on_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ahl7f3</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Tropic low</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahl7f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ahkahx</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Death Valley Nails brush is trash and I was Not expecting that</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahkahx/death_valley_nails_brush_is_trash_and_i_was_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ahk9mb</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>3 and a half hours later…</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahk9mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ahk12o</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>First time in a long time!</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahk12o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1ahju6z</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Recovering 30 year nail biter</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahju6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1ahjjpn</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Sales that I should put in my calendar?</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahjjpn/sales_that_i_should_put_in_my_calendar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1ahjeq9</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>A tragedy has befallen my glass file. Anybody just carry on using what’s functionally left, or do I need to see clearly here and buy a replacement?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs8n1ao0q9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ahject</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Sassy Sauce - Cock-a-doodle-doom</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahject</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1ahj9sw</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>finally had to chop these babies down and was sad but a new color always makes it easier!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahj9sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ahj6i2</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>LynBDesigns | Dudley Nudshite + Monarch Lacquer | Belladonna</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbfiiem0o9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ahj54t</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Treat yo’ self purchases</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahj54t/treat_yo_self_purchases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ahj33i</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>My February Nails</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahj33i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ahiowz</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Pre-Valentines Mani, Arwen+Aragorn</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahiowz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ahidsn</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>What A Pansy by China Glaze</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v8prk7dh9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ahhwkj</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>I guess I thought it had a blackish base? Pretty disappointed. Now I have to do 2 black/colored coats, then like 4 of this? This is three coats!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y89xdcld9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ahhmis</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>I’m newer to indie polish. ELI5</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahhmis/im_newer_to_indie_polish_eli5/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ahhdjb</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>My nail polish choices for a trip back home.</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51fbry6h99gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ahh62j</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Valentine's mani!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahh62j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ahguxt</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>why are my nails curling down like this when they grow?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6624w6vh59gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ahgur5</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>So disappointed in myself. I bit off my long natural nails due to a stressful visit with extended family. I don't know what happened, I never bite my nails. Anyway, join me in mourning my once beautiful long natural nails.</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyirw6f659gc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ahgkyb</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>🌺 BKL Maui + ILNP Atlantis 🌊</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n4hdxlad39gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ahgb9s</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Was forced into a short square shape by my washing machine… but I can’t get mad at that perfect break.</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz3h3dad19gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ahfzhi</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>{PR} Red flakies 😍</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71wjl66wy8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ahcir8</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>I knew saving these boxes would come in handy</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhmjxiuk88gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ahf1om</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>January 2024 - Mani Log and Review!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahf1om</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1aheg6z</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>My First Flakie 💕</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ioums736n8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ahefk5</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>The Slickest of Them All</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahefk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ahe6rs</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Mooncat Velvet Rose</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahe6rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ahe0zi</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>rogue - glowy af 🤩🤩🤩</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahe0zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ahdzsy</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Curfew Crasher</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahdzsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ahde3w</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Swatches of some new purchases/deciding which to wear…</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq6qqfg9f8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ahcu44</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Waiting in the vehicle service center ✨ lighting ✨</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97px5dvxa8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ahcmu6</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Love is in the air ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bdon5cf98gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ahcm2i</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>A super fun polish ft maybe a little trypophobia?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahcm2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ahcgrc</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Used a scented QDTC for my swatches</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbgnzzw588gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ahcbnv</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>How would you make my kid's dream of matching Lightning McQueen nails a reality?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahcbnv/how_would_you_make_my_kids_dream_of_matching/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ahc1ja</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Recommendations for Contrast Shimmers or Shifts in Brown/Neutral?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahc1ja/recommendations_for_contrast_shimmers_or_shifts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1ahbneu</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Chrome powder on polish/lacquer?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahbneu/chrome_powder_on_polishlacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1ahbn7h</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Swatch comparison: Ether Dragon, Now Go and Don't Look Back, LSD.</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahbn7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1ahbasb</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Fun with metallic green 😊</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/sZIjEIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ahas1c</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Pink Skittle with Shifty Topper</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahas1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ahalsd</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Beach of Singing Sands</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahalsd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ahahcg</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>🌙🪽🌆</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahahcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1ahaa2r</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Need a SERIOUS ridge filling base coat that I can put multiple coats of on if needed.</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahaa2r/need_a_serious_ridge_filling_base_coat_that_i_can/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ah9uw1</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>LynB- Catch My Drift from “Winter Customs”</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0eipbs4ho7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ah9oql</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>A Dainty Mani</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah9oql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ah8t5p</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Random Combo</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/725pewyig7gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ah8pbc</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Encore by h&amp;m is my new favorite</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aemewbupf7gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ah8ic4</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Looking for similar polishes</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z28sv0j9e7gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ah89dg</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Now Go and Don’t Look Back 🤩</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2b7fbkigc7gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ah82ua</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Zoya Sasha</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah82ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ah7zub</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Paradox Polish - Wisteria</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah7zub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ah7ub1</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>“Do you think I’m spooky?”</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m47pasxb97gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ah7j2m</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>My first thermal!</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/78fipnww67gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ah6sxf</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Regrets?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imeir0yf17gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ah6guk</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>I used this bookcase my Dad built in the 90's for his CD collection to display my Holo Taco collection 💿🌮💅🏻🥰</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qunwf5qy6gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ah6g0p</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Mishipeshu (the great lynx)</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah6g0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ah67b7</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>A Dragon Without A Rider Is A Tragedy 🐉</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6eq4xo6iw6gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ah5h3j</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>I love this combo! Take Me to Your Leader by Mooncat topped with Flakie Holo Taco by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah5h3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ah46lf</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Welp, apparently this is a peely base</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ah46lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1ah1uqp</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>OPI Nail Envy new formula</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ah1uqp/opi_nail_envy_new_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ah1bnk</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Looking for a bright, opaque white.</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ah1bnk/looking_for_a_bright_opaque_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ahqv4i</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Does anyone have a tutorial or can advise for how to do the circled nails with gel polish? The swirly red and pink ones.</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e69lnr68sbgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ahqqhe</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>How To Make Juicy Ombre💛💚</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pxkplwlqbgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ahn7n1</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Submissive Themed Gel Set (Nude/Black/Gold)</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhvmftmyoagc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ahlqd7</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Sailor Moon inspired nails by Shauntelle Hubbard at Shear Mellegence salon in Radford, VA</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hwr9gnrxaagc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ahkxoo</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60e8f9qn3agc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ahj2zi</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>I think I hate them &lt;/3</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahj2zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ahi9nb</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>two designs i did today</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahi9nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ahhote</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>My BIL's girlfriend and I got a Valentine's Day set done a little early. I love them both 🫶</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1877halwb9gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ahhf2x</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>First nail art</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t8p4lgs99gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ahh6dy</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Kept it simple for Valentines this year</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol40f0ox79gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ahf4a3</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>This nail charm is MASSIVE 😅</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ywl96g9s8gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ah8au6</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Dragon’s Egg Nails</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v11e3fpqc7gc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ah1yhu</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>All you need is love ❤️</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmvcambbv5gc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb  4 08:06:54 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_04.xlsx
+++ b/data/2024_02_04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1119"/>
+  <dimension ref="A1:C1316"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19456,6 +19456,3355 @@
         </is>
       </c>
     </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1aiiq35</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Stickers can really pull a look together quick 💗</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aiiq35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1aiin59</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>which set should I get for the next time</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aiin59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1aihtrj</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>The prettiest shade 😊</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vldeucstnigc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1aihmq5</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Im a self taught nail tech &amp; I just did this set on my bestfriend what do you think? Honest critique is more then welcomed &amp; I definitely won’t take any offense if there’s things I can work on to perfect my craft 🥰</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvj1vp6mligc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1aih00g</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Cute</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnb0rbhleigc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1aifisr</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>[Help] Gel manicures in Europe and gel manicures in the US are different! I can't figure out how to get the European version in the US, but that one lasted SO long. Does anyone know what "UV gel" is in the US?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aifisr/help_gel_manicures_in_europe_and_gel_manicures_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1aidynm</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0insaryjhgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1aifp0i</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Making press ons as a pottery girly (playing with 3D gel)</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aifp0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1aibn4f</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>How to fix indents on nail</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aibn4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1aifd7d</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>New press on set 🤍</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aifd7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ai9fgy</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Nails inspo for mom who bites her nails</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai9fgy/nails_inspo_for_mom_who_bites_her_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ai8r0r</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Discoloration around edges 3 days after gel mani - too picky?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njbsvxoqaggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ai8h8o</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Found the idea from Pinterest. What do yall think?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijkbjixj8ggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1aif6fh</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Press on twinsies!</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aif6fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1aif5jf</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Pink is my favourite colour😍 pearly valentines nails💟</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aif5jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1aiev7c</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>My nail tech did excellent work on my art deco styled set!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aiev7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1aieu3u</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>I'm obsessed with chrome nails 🌟</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awgb5qzeshgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1aieqmr</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Are these realistic results or fake? Done by @andreadesignernf on IG</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aieqmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1aie4ys</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>New set 💕💗</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aie4ys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1aie0ec</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Just wanted to share my Valentine’s nails 💅🏼💗</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ug07e4ffkhgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1aidlku</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Valentine's day set ordered by a mother and her two daughters</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aidlku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1aidfao</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/habkcu5yehgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1aid6fq</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>My nail tech is a miracle worker</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0s3zpfmchgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1aicqui</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Is it possible that my Russian manicure has made my cuticles worse?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aicqui/is_it_possible_that_my_russian_manicure_has_made/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1aicpp2</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Loving my festive nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f8cxyoc8hgc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1aicjrb</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Can this crack be stabilized with a gel mani or should I just bite the bullet and cut it?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aicjrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1aicd12</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My Feb nails! 🍒♥️</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aicd12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1aic5h1</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Ready for a day of love!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz53gom83hgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1aibw05</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>I finally got my Valentine’s Day set! ♥️💗🤍</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfc5hywv0hgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1aibucn</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>First-ever Holo Taco order, so of course I had to try them all at once (I’m new here so don’t roast me… or do, idk)</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aibucn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1aibft9</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>I see fill recommended every two to three weeks?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5spxydwwggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1aiaqgo</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Tried the magnetic heart nails!</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gd3seruqggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1aiamgi</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Found some Snoopy nail stickers and did my mom's nails</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbn2umowpggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1aia3pn</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Valentines vibes have begun 💕</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jglb24fmlggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ai74yz</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Second ever set of nails</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai74yz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1aia2m4</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>(Male) Dark blue and dark green</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aia2m4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ai6ihp</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Alternatives to acrylic?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai6ihp/alternatives_to_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ai5n5b</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>In Love !!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai5n5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ai4b0t</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>which nail shape would be best?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai4b0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ai3a4u</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Opinions?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai3a4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ai9rh9</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Valentine set 🖤💕</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j7mrjvuiggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ai09l9</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Done by my classmate (we’re soon to be nail techs🥰🥰) including inspo taken from @douxnailsbb on instagram</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai09l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ai9qab</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>black valentine’s day nails 🖤</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoz8co0liggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ai90o4</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>press ons 🤌🏼</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jh6aewdvcggc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ai8xa4</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Yes? No? Valentine's nails I just had done</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myexcia4cggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ai8v6r</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>How are my nails? First time poly gel! I was so high while doing this.</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai8v6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1ai8rfo</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Reposting due to my post being removed :/ hope you like! Sorry they’re not brand new like when I posted but hope you still like them.</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai8rfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1ai8r0m</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Really happy with this set</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w285ewsqaggc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1ai8d0y</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>French Kiss Manicure 😘💋</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ffsxczl7ggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1ai8bih</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>What order should I be using products</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai8bih/what_order_should_i_be_using_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ai7zeb</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Will this work as nail oil?</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0d0oxlj4ggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ai7xv0</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Red Stars ft cool rings and my crooked fingers</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai7xv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ai7mu5</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Birthday nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg3rpaju1ggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ai7kgo</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Would a normal paint brush for painting work for nail art?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai7kgo/would_a_normal_paint_brush_for_painting_work_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ai7iun</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Second set I’ve ever done on real hands</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4obr5ox0ggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ai7cqw</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Winter Holiday Manicure</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai7cqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ai6wgg</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Did my mom's Valentines nails!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6wgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ai6vwm</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6vwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ai6odq</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Valentine’s day nails 💅🏻 🩷</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b7na9oq9ufgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ai6mq2</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Just got my nails done! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6mq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ai6hea</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Holiday nails ☀️ These took my nail girls 2.5 hours which seems very long - is this standard?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vrawa3ssfgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ai6h8z</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>🩷</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6h8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ai6h5q</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Tiramisu for Two</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6voxnbqsfgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ai6594</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Would it be a good idea to use superglue for my acrylics</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7u3qqp1qfgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ai613b</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Some peachy-chrome press ons this week. Short for work purposes but I still like ‘em.</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai613b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ai60s2</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>how to fix design on gel nails after cured top coat?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai60s2/how_to_fix_design_on_gel_nails_after_cured_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ai5xiq</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Carrie 🩸</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whs9w4ufofgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ai5vo6</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>How can I use these stickers?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klvd6771ofgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ai5rur</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>My first visit to a brand new opened Nail Saloon in my neighborhood. I am fuming😭</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai5rur</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ai5fzb</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>How many days will Sally Hansen Miracle Gel tend to last?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai5fzb/how_many_days_will_sally_hansen_miracle_gel_tend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ai56n8</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai56n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ai54uj</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>What shape would be best for my nails?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai54uj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ai4tfv</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>be honest!! I was hoping the base color would be a little more sheer; do we like these anyway!? 🤣🥰</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uornii2nffgc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ai4rf1</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>French tips i painted first attempt</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai4rf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ai3t5v</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>I did it in one hour!</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1mzlczn7fgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1ai3qec</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Did my Nails today at the Salon</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai3qec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ai3emn</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Should you tip for needing to get a dip manicure fixed?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai3emn/should_you_tip_for_needing_to_get_a_dip_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ai3e5w</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Happy early Valentine’s Day! How much would you pay / charge for this set?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/633y5jda4fgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ai36va</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Throwing in Snoopy made me happy 🐶</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ovzyj3o2fgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ai2ywm</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Ex Nail biter BIAB journey just beginning</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai2ywm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ai2s74</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>First time using poly gel</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48fyyrlgzegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1ai2l9f</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Waiting After Nails are Done (etiquette question)</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai2l9f/waiting_after_nails_are_done_etiquette_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1ai2kde</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Decided to go simple for Valentine’s Day… how did I do?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjnwh4pqxegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ai2iwk</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Valentine’s Sweater Vibes</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nl2v2eeexegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ai2icf</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Pink and glittery for Valentine’s 🩷</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozxjtbw9xegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ai25fu</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>6 Months of Doing My Own Nails</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai25fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1ai2527</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Acrylic overlay on natural nails. Growth from Dec 9 2023 - Feb 2 2024</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai2527</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ai1psg</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>The beetles Gel X kit is bomb</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfl801c3regc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1ai1muh</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>I haven't had a French done since the early 2000's! I'm so glad they're making a comeback!</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai1muh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ai1h2l</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Valentines day nails❤️💅🏼</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11t88qo7pegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ai1bam</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>my hello kitty set🎀</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai1bam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ai10x8</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Cutest Valentine’s Day shorties! Structured manicure hard gel overlay ♥️</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/os4znh8nlegc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ai10mq</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Natural Russian manicure 🤍💅🏻</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai10mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ai0y42</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>One of my favorite mani’s😍💅🏻</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai0y42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ai0uvz</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Russian Manicure💅🏻</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai0uvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ai0szj</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Russian manicure - my fav past Mani’s 😍💅🏻</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai0szj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1ai0se9</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>"The continual and eternal knot is everlasting and unbreakable" 🩷</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai0se9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1ai0sas</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>I want to practice using nail polish</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ai0sas/i_want_to_practice_using_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1ai0ros</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>did press on nails first-time.</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om6l4fepjegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1ai0n48</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Valentine nails last year ❤️</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxpenoqriegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1aif9vx</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Emily De Molly Small Movements</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aif9vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1aih77e</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Loving the new kiss nails! They glisten a ton in the sunlight!</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aih77e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1aigsrq</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Blue Green Mood</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfba1ythcigc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1aigp34</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Romance</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aigp34</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1aifuc1</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Phoenix - Boolba</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aifuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1aifmqt</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Are they classy or childish? I can’t tell 😩</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7ped23d0igc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1aifl5u</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Varicose Veins</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9tmk4m6zhgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1aif8hm</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Miss these opals already</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq9ng7ddwhgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ai8aj7</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>First time trying ILNP</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai8aj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1aif2b8</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqbioqonuhgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1aier4x</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>❤️Elmo❤️</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aier4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1aieg2o</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>mystic moonstone french manicure</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aieg2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1aie4jl</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Lights Lacquer swatches!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aie4jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1aidtgo</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Favorite ILNP polish? (Pics or without)</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aidtgo/favorite_ilnp_polish_pics_or_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1aidni9</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Chinese new year nails!🐉</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d39thi03hhgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1aid0dh</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Donated all my gel polish and supplies today</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aid0dh/donated_all_my_gel_polish_and_supplies_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1aibojm</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>finally pulled my collection together and i’m so happy</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aibojm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1aib6mo</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Mooncat Artemis’ Deathkiss &amp; Holo Taco Scorched Earth</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aib6mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1aib1i5</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>my boyfriend doesn’t like my nails</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8uyfxyftggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1aiall1</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>why do these 2 nails always break?😭</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgtdoc7ppggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1aiakf1</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Her Dark Majesty 🖤</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aiakf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1aiaeli</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>What color to add to make this a better nude pink on me?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqap8t12oggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1aiaazj</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Swatching!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aiaazj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1aia54z</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>DRK Azalea</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aia54z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1aia02k</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First velvet nails attempt </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1xhn6g7qkggc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ai9z11</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Damn it Janet</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai9z11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ai9dus</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>French, but make it sparkly ✨️</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai9dus</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1ai99ip</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day mani featuring the only milky pink I’ve tried that wasn’t a nightmare to apply! Akzentz Luxio Afterglow</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai99ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ai8y74</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Please look at my mom’s adorable pinky!!!</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai8y74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1ai8lmw</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I cannot stop staring at my nails!</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/96vdmwoi9ggc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1ai81bi</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Attempt 1 match the ring!</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai81bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1ai7y9r</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Casual post - unboxing</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bv9zjoe94ggc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1ai7qxa</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>first valentine manicure 💌</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai7qxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1ai7qm5</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>V-Day Challenge: Mani #2</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai7qm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1ai73dv</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>The Love Spell has been casted!</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai73dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1ai71yq</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>How do I achieve this with gels?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7kljsd9xfgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1ai6wph</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Been thinking about trying this combo for awhile!!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6wph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1ai6u8e</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Mooncat - Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6u8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1ai6ry9</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Yeah, went a bit crazy....</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6ry9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1ai6p19</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Nude/neutral polish suggestions?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6p19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1ai6fqi</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>I couldn't decide...</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6fqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1ai6ce6</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>French manicure with regular polish</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ai6ce6/french_manicure_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1ai5z33</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Life long nail biter, until now!</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1dbnqyrofgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1ai5v90</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Carrie 🩸</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9jmy98ynfgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1ai5nd0</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>One of the many faces of Now Go and Don’t Look Back</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7j2bcg9mfgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1ai56oc</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Cleaning out my storage closet and found some gems I thought I threw out years ago! 😍</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zptujovjifgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1ai552a</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Semi translucent pink gel polish</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u16djh97ifgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1ai4irw</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>First time trying Kiss press ons and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grco4nnadfgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1ai464n</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Fake halo in direct sunlight is just angelic 😇</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai464n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1ai3umg</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>My first LynB order and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai3umg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1ai3508</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Mooncat Sand Viper</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyfykly92fgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1ai31nz</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Organized my Mooncat collection</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kg8m9hj1fgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1ai2sc9</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Tried stickers for the first time</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbcjzfohzegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1ai2nsf</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Head in the clouds by Moon Cat 🌙 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai2nsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1ai2man</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Can’t believe I used to sleep on multichromes</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elpalcu5yegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1ai2got</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Okay, I LOVE Boolba 🥹</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai2got</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1ai1sar</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Ether Dragon + Dahlia</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai1sar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1ai1qx3</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Pre-Valentine's mani 🩷</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujwrfrscregc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1ai11x1</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Spring Floral nails 🥹</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai11x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1ai0zif</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Expect more from thermals!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai0zif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ai0snk</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Lilacquer 🙃</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/5lr6n3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ai0mf1</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Valentine’s set for daughter</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4h6zj0fmiegc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ai0cqk</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>First Holo Taco order as I’m on the hunt for my perfect purple 💜</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai0cqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ai0blq</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Velvet Venom</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0c2drpe5gegc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1ai084y</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Feed Me!</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai084y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1ahzy0b</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>One day, I’ll be able to photograph holographic polish</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gmjqvx8degc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1ahznep</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>how do yall remove dnd polish?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahznep/how_do_yall_remove_dnd_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1ahz83f</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Don’t go bacon my heart 🐷❤️</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahz83f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1ahz1q9</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Anyone know of an alternative to OPI Repair Mode?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ahz1q9/anyone_know_of_an_alternative_to_opi_repair_mode/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1ahz0ix</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Velvet Rope is so warm and glowy 😍</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6e2obxfv5egc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ahye0t</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>No more regrets!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahye0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ahxbjy</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Y’all were right!!! FIVE days wear with proper prep + basecoat + topcoat. Emily de Molly Written Invitation</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahxbjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1ahx23s</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>When the vision and execution don't quite match</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahx23s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ahwcse</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Note to self-don’t use a peely base if I’m going to be kneading bread dough 🥴</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkxy53d9jdgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1ahwals</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>What are your favorite cool tone polishes?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5l01drlidgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1ahvyrg</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Nails based on one of my favorite book series/ shows also happen to be perfect for Valentines Day</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8bexkqdfdgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1ahvnsz</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Another neutral with a twist!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahvnsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1ahvcky</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>airbrush and chrome always go well together! handpainted by me! (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbv7nyek9dgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ahuvoo</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>First Skittles - Fell into the Nail Polish Rabbithole two weeks ago</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahuvoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1ahtl8i</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>My first order of indie nail polish ✨💙</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahtl8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ahtcqm</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>My “I’m heartbroken and don’t like Valentine’s Day” pre-Valentine’s Day mani 🙃</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55rfgbnrmcgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1ahsow0</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Older set, inspired by a post from this sub.</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahsow0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1ahra1l</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Favorite combo I’ve done so far and perfect for Valentines Day 💕 (see comments for link to video)</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va91shd7xbgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1ahr7oi</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>One of my favorites 🥹🩵🏞️</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahr7oi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1aihu4v</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>:(</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1aihu4v/_/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1aigfne</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>My first ever pop art style that glows in dark</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aigfne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1aiedkz</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Birthday trip nails</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aiedkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1aib25q</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>This is officially the hardest thing Ive ever done in my entire life.</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otqex6qltggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1ai9jnn</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>🍌🫣</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wjw8jl2hggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1ai8l77</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>First try with gel</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7kbssod9ggc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1ai8g9x</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Early Valentine’s Day nails 💖</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5haacmb8ggc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1ai87tn</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Love is Scary 💅🏻⛈️💖🔪💌🔥🥀</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai87tn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1ai6vr8</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Did my mom's valentines nails!</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ai6vr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ahzl0m</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>I'm absolutely in love with my work today 💙</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahzl0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ahwm2k</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>💕💕💕</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ahwm2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ahv9li</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Today I did these nails with striations and I loved how they turned out.</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvg9wlyo8dgc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ahsyp7</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Pop-art cell shaded on my natural nails by @kalsrebelliousnails on IG in Seattle</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78h9g0imhcgc1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>